<commit_message>
Changed grade calc picture
</commit_message>
<xml_diff>
--- a/grade-calc-template.xlsx
+++ b/grade-calc-template.xlsx
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>